<commit_message>
Finished first draft of Import page
</commit_message>
<xml_diff>
--- a/Files/Data/ExampleXLSX.xlsx
+++ b/Files/Data/ExampleXLSX.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RStudio\Projects\RTraining\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RStudio\Projects\TQLTraining\Files\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F4707F0-6D88-4CA3-8201-8B4B7739EE5D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{964690D9-B10B-475B-9593-CA776B312A69}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="12360"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="28800" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ExampleCSV" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>Col1</t>
   </si>
@@ -43,19 +44,28 @@
     <t>F</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Character</t>
-  </si>
-  <si>
-    <t>Variable</t>
+    <t>This</t>
+  </si>
+  <si>
+    <t>Sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number </t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Two</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -889,10 +899,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E4EFC3B-084A-4093-8843-0BF5D0216EC3}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -912,7 +924,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -934,7 +946,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -945,7 +957,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -956,7 +968,88 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>

</xml_diff>